<commit_message>
This time I mean it
</commit_message>
<xml_diff>
--- a/Timing Category.xlsx
+++ b/Timing Category.xlsx
@@ -343,7 +343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -404,7 +404,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Prediction</t>
+          <t>Forecast</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
@@ -477,16 +477,6 @@
           <t>Other</t>
         </is>
       </c>
-    </row>
-    <row outlineLevel="0" r="10">
-      <c r="A10" s="0"/>
-      <c r="B10" s="0" t="inlineStr"/>
-      <c r="C10" s="0" t="inlineStr"/>
-    </row>
-    <row outlineLevel="0" r="11">
-      <c r="A11" s="0"/>
-      <c r="B11" s="0" t="inlineStr"/>
-      <c r="C11" s="0" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>